<commit_message>
Additional Columns and button
</commit_message>
<xml_diff>
--- a/bin/Debug/Template/SparePartBalance.xlsx
+++ b/bin/Debug/Template/SparePartBalance.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT-Project\MC-Dept-App\bin\Debug\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT06-PC\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31437D0E-14AB-4351-91FC-63A11539545F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3466D046-C4AC-4750-BB6A-0ADE1D91D688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5C9B76C0-C1B0-491E-AA96-3260EA1B797B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$N$2</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -88,10 +91,12 @@
       <b/>
       <sz val="20"/>
       <color theme="9"/>
-      <name val="Khmer OS"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -101,12 +106,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -149,14 +148,14 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -495,13 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE271FD4-1BA6-4BFE-B7DF-1A8BDD361B8D}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,8 +515,8 @@
     <col min="14" max="14" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5"/>
@@ -595,9 +591,10 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="4"/>
+      <c r="N3" s="6"/>
     </row>
   </sheetData>
+  <autoFilter ref="A2:N2" xr:uid="{EE271FD4-1BA6-4BFE-B7DF-1A8BDD361B8D}"/>
   <mergeCells count="1">
     <mergeCell ref="A1:N1"/>
   </mergeCells>
@@ -610,6 +607,5 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="43" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revise balnce search and print Po request
</commit_message>
<xml_diff>
--- a/bin/Debug/Template/SparePartBalance.xlsx
+++ b/bin/Debug/Template/SparePartBalance.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT06-PC\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT-Project\MC-Dept-App\bin\Debug\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3466D046-C4AC-4750-BB6A-0ADE1D91D688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3364CB3C-EB6D-4D5C-A6B9-F8E000685FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5C9B76C0-C1B0-491E-AA96-3260EA1B797B}"/>
   </bookViews>
@@ -16,7 +16,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$N$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$P$2</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$P$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Spare Part Balance</t>
   </si>
@@ -73,12 +74,21 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Balance Order</t>
+  </si>
+  <si>
+    <t>Plan ETA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mmm/yyyy"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -110,7 +120,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -133,11 +143,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -148,14 +178,18 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -494,10 +528,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE271FD4-1BA6-4BFE-B7DF-1A8BDD361B8D}">
-  <dimension ref="A1:N3"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection sqref="A1:P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,27 +550,31 @@
     <col min="12" max="12" width="10.85546875" customWidth="1"/>
     <col min="13" max="13" width="17.7109375" customWidth="1"/>
     <col min="14" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" customWidth="1"/>
+    <col min="16" max="16" width="20.7109375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
     </row>
-    <row r="2" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -576,8 +617,14 @@
       <c r="N2" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="O2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -591,14 +638,16 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="6"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:N2" xr:uid="{EE271FD4-1BA6-4BFE-B7DF-1A8BDD361B8D}"/>
+  <autoFilter ref="A2:P2" xr:uid="{EE271FD4-1BA6-4BFE-B7DF-1A8BDD361B8D}"/>
   <mergeCells count="1">
-    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A1:P1"/>
   </mergeCells>
-  <conditionalFormatting sqref="N3">
+  <conditionalFormatting sqref="N3:P3">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="No Order">
       <formula>NOT(ISERROR(SEARCH("No Order",N3)))</formula>
     </cfRule>
@@ -607,5 +656,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="37" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>